<commit_message>
Add link to Notes
</commit_message>
<xml_diff>
--- a/Notes & How to Do's.xlsx
+++ b/Notes & How to Do's.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Working Repo\JS Sketches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Working Repo\JS Sketches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C031E65-C15C-4AA1-9869-12D66B2B2CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC853B86-AE17-4FEE-A765-0A5C7A1B3E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Canvas Sketch</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Canvas API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.npmjs.com/package/simplex-noise </t>
+  </si>
+  <si>
+    <t>Noise Algorithm</t>
   </si>
 </sst>
 </file>
@@ -540,15 +546,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836BF3A2-9612-4E19-8A5A-39B85B2C4DE6}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
     <col min="2" max="2" width="108.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -733,12 +739,21 @@
         <v>43</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B29" r:id="rId1" xr:uid="{46A19F64-349A-44B0-A74F-1FC74B607EC3}"/>
+    <hyperlink ref="B30" r:id="rId2" xr:uid="{4CDE2ADA-094B-4694-9A36-DFC36D6CB1CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Implemented GUI using Tweakpane
Installed various sliders to manipulate sketch by allowing the using to use the GUI to change variables & parameters on the fly. To explore uses in previous sketches and future ones
</commit_message>
<xml_diff>
--- a/Notes & How to Do's.xlsx
+++ b/Notes & How to Do's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Working Repo\JS Sketches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF471517-2543-43B5-A2EA-F2B4348639A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D516AE-DDDF-4EC0-84EC-1E341321FC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Canvas Sketch</t>
   </si>
@@ -182,6 +182,24 @@
   </si>
   <si>
     <t>canvas-sketch sketch-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cocopon.github.io/tweakpane/ </t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>npm i tweakpane</t>
+  </si>
+  <si>
+    <t>To Install (npm)</t>
+  </si>
+  <si>
+    <t>For setting up input sliders &amp; GUI input that can be customised</t>
+  </si>
+  <si>
+    <t>Installs tweakpane using npm</t>
   </si>
 </sst>
 </file>
@@ -552,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836BF3A2-9612-4E19-8A5A-39B85B2C4DE6}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -695,7 +713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -703,12 +721,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -716,12 +734,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -729,7 +747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -737,7 +755,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -745,7 +763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -753,21 +771,44 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B29" r:id="rId1" xr:uid="{46A19F64-349A-44B0-A74F-1FC74B607EC3}"/>
     <hyperlink ref="B30" r:id="rId2" xr:uid="{4CDE2ADA-094B-4694-9A36-DFC36D6CB1CD}"/>
+    <hyperlink ref="B31" r:id="rId3" xr:uid="{AACC4D29-C5C6-4959-9744-CF22B1BCEAE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Set up new Laptop
</commit_message>
<xml_diff>
--- a/Notes & How to Do's.xlsx
+++ b/Notes & How to Do's.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Working Repo\JS Sketches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Working Repo\JS Sketches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB7532-436C-4B34-8EAF-A6EC03BF8CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864A0B23-FBBA-4DC3-BD1C-348B1C2677BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Canvas Sketch</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Clears screen</t>
   </si>
   <si>
-    <t>in cmder type, npm install canvas-sketch to install canvas sketch</t>
-  </si>
-  <si>
     <t>in cmder type npm update, updates all npm packages</t>
   </si>
   <si>
@@ -206,13 +203,40 @@
   </si>
   <si>
     <t>To check</t>
+  </si>
+  <si>
+    <t>npm install canvas-sketch-util --save</t>
+  </si>
+  <si>
+    <t>npm install canvas-sketch --save</t>
+  </si>
+  <si>
+    <t>in cmder type, the following to install packages</t>
+  </si>
+  <si>
+    <t>npm install tweakpane --save</t>
+  </si>
+  <si>
+    <t>npm install canvas-sketch-cli -g</t>
+  </si>
+  <si>
+    <t>Need this for cmdr to work, won't recognise canvas-sketch without it</t>
+  </si>
+  <si>
+    <t>webstorm</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + L</t>
+  </si>
+  <si>
+    <t>Reformat Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,6 +255,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -256,11 +287,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -576,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836BF3A2-9612-4E19-8A5A-39B85B2C4DE6}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -638,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -649,7 +682,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -674,36 +707,36 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -721,106 +754,119 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
         <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
         <v>39</v>
       </c>
-      <c r="B24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
         <v>52</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1" xr:uid="{46A19F64-349A-44B0-A74F-1FC74B607EC3}"/>
-    <hyperlink ref="B30" r:id="rId2" xr:uid="{4CDE2ADA-094B-4694-9A36-DFC36D6CB1CD}"/>
-    <hyperlink ref="B31" r:id="rId3" xr:uid="{AACC4D29-C5C6-4959-9744-CF22B1BCEAE6}"/>
-    <hyperlink ref="B33" r:id="rId4" xr:uid="{A6D784E6-FA7B-44B9-BD77-86B1D9D13F48}"/>
+    <hyperlink ref="B30" r:id="rId1" xr:uid="{46A19F64-349A-44B0-A74F-1FC74B607EC3}"/>
+    <hyperlink ref="B31" r:id="rId2" xr:uid="{4CDE2ADA-094B-4694-9A36-DFC36D6CB1CD}"/>
+    <hyperlink ref="B32" r:id="rId3" xr:uid="{AACC4D29-C5C6-4959-9744-CF22B1BCEAE6}"/>
+    <hyperlink ref="B34" r:id="rId4" xr:uid="{A6D784E6-FA7B-44B9-BD77-86B1D9D13F48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -829,45 +875,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D3260A-B611-42E4-9480-81339A67FCC9}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial Commit for PaperOwlz
</commit_message>
<xml_diff>
--- a/Notes & How to Do's.xlsx
+++ b/Notes & How to Do's.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Working Repo\JS Sketches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Working Repo\JS Sketches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864A0B23-FBBA-4DC3-BD1C-348B1C2677BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D88452-8B31-4834-8961-20725208331F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{58412012-68BF-40B6-8AE5-8C9A9DEAED96}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -878,7 +878,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>